<commit_message>
trim data & change model
</commit_message>
<xml_diff>
--- a/release/obligations.xlsx
+++ b/release/obligations.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Description*</t>
   </si>
   <si>
     <t xml:space="preserve">Type*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institution</t>
   </si>
   <si>
     <t xml:space="preserve">Remaining Balance</t>
@@ -38,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">Monthly Payment*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day of Month</t>
   </si>
 </sst>
 </file>
@@ -170,26 +164,130 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G995"/>
+  <dimension ref="A1:G965"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -200,30 +298,20 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="7"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="7"/>
@@ -3114,99 +3202,9 @@
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B965" s="7"/>
     </row>
-    <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B966" s="7"/>
-    </row>
-    <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B967" s="7"/>
-    </row>
-    <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B968" s="7"/>
-    </row>
-    <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B969" s="7"/>
-    </row>
-    <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B970" s="7"/>
-    </row>
-    <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B971" s="7"/>
-    </row>
-    <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B972" s="7"/>
-    </row>
-    <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B973" s="7"/>
-    </row>
-    <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B974" s="7"/>
-    </row>
-    <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B975" s="7"/>
-    </row>
-    <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B976" s="7"/>
-    </row>
-    <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B977" s="7"/>
-    </row>
-    <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B978" s="7"/>
-    </row>
-    <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B979" s="7"/>
-    </row>
-    <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B980" s="7"/>
-    </row>
-    <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B981" s="7"/>
-    </row>
-    <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B982" s="7"/>
-    </row>
-    <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B983" s="7"/>
-    </row>
-    <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B984" s="7"/>
-    </row>
-    <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B985" s="7"/>
-    </row>
-    <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B986" s="7"/>
-    </row>
-    <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B987" s="7"/>
-    </row>
-    <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B988" s="7"/>
-    </row>
-    <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B989" s="7"/>
-    </row>
-    <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B990" s="7"/>
-    </row>
-    <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B991" s="7"/>
-    </row>
-    <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B992" s="7"/>
-    </row>
-    <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B993" s="7"/>
-    </row>
-    <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B994" s="7"/>
-    </row>
-    <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B995" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B995" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B965" type="list">
       <formula1>"Loan,Credit Card,Bill,Expense"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>